<commit_message>
Bugs fixed - stable release
</commit_message>
<xml_diff>
--- a/public/Updatedtranslations.xlsx
+++ b/public/Updatedtranslations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="788">
   <si>
     <t>English</t>
   </si>
@@ -1777,6 +1777,12 @@
     <t>من حيث الموقع والمكون</t>
   </si>
   <si>
+    <t>Late In, Early Out</t>
+  </si>
+  <si>
+    <t>متأخرًا في وقت مبكر للخروج</t>
+  </si>
+  <si>
     <t>welcome Back!: "مرحبا بعودتك!",</t>
   </si>
   <si>
@@ -2372,9 +2378,6 @@
   </si>
   <si>
     <t>From recruitment to retirement, manage every employee journey seamlessly and efficiently.</t>
-  </si>
-  <si>
-    <t>Late In, Early Out</t>
   </si>
 </sst>
 </file>
@@ -5235,7 +5238,14 @@
         <v>586</v>
       </c>
     </row>
-    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1">
+      <c r="A314" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="B314" s="6" t="s">
+        <v>588</v>
+      </c>
+    </row>
     <row r="315" ht="15.75" customHeight="1"/>
     <row r="316" ht="15.75" customHeight="1"/>
     <row r="317" ht="15.75" customHeight="1"/>
@@ -5947,7 +5957,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B1" s="11" t="str">
         <f t="shared" ref="B1:B197" si="1">TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LEFT(A1, FIND(":", A1) - 1), """", ""), "'", ""), ",", ""))</f>
@@ -5960,7 +5970,7 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B2" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5973,7 +5983,7 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B3" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5986,7 +5996,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B4" s="11" t="str">
         <f t="shared" si="1"/>
@@ -5999,7 +6009,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B5" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6012,7 +6022,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B6" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6025,7 +6035,7 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B7" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6038,7 +6048,7 @@
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B8" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6051,7 +6061,7 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B9" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6064,7 +6074,7 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B10" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6077,7 +6087,7 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B11" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6090,7 +6100,7 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B12" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6103,7 +6113,7 @@
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B13" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6116,7 +6126,7 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B14" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6129,7 +6139,7 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B15" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6142,7 +6152,7 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B16" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6155,7 +6165,7 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B17" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6168,7 +6178,7 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B18" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6181,7 +6191,7 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B19" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6194,7 +6204,7 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B20" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6207,7 +6217,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B21" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6220,7 +6230,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B22" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6233,7 +6243,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B23" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6246,7 +6256,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B24" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6259,7 +6269,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B25" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6272,7 +6282,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B26" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6285,7 +6295,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B27" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6298,7 +6308,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B28" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6311,7 +6321,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B29" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6324,7 +6334,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B30" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6337,7 +6347,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B31" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6350,7 +6360,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B32" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6363,7 +6373,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B33" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6376,7 +6386,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B34" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6389,7 +6399,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B35" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6402,7 +6412,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B36" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6415,7 +6425,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B37" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6428,7 +6438,7 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B38" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6441,7 +6451,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B39" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6454,7 +6464,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B40" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6467,7 +6477,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B41" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6480,7 +6490,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B42" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6493,7 +6503,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="11" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B43" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6506,7 +6516,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="11" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B44" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6519,7 +6529,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B45" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6532,7 +6542,7 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B46" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6545,7 +6555,7 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B47" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6558,7 +6568,7 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="11" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B48" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6571,7 +6581,7 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="11" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B49" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6584,7 +6594,7 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B50" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6597,7 +6607,7 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="11" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B51" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6610,7 +6620,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="11" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B52" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6623,7 +6633,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="11" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B53" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6636,7 +6646,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="11" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B54" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6649,7 +6659,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="11" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B55" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6662,7 +6672,7 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="11" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B56" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6675,7 +6685,7 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="11" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B57" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6688,7 +6698,7 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="11" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B58" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6701,7 +6711,7 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="11" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B59" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6714,7 +6724,7 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="10" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B60" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6727,7 +6737,7 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="11" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B61" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6740,7 +6750,7 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="10" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B62" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6753,7 +6763,7 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="11" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B63" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6766,7 +6776,7 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="11" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B64" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6779,7 +6789,7 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="11" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B65" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6792,7 +6802,7 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="11" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B66" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6805,7 +6815,7 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B67" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6818,7 +6828,7 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="11" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B68" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6831,7 +6841,7 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="11" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="B69" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6844,7 +6854,7 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="11" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B70" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6857,7 +6867,7 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="11" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B71" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6870,7 +6880,7 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="11" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B72" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6883,7 +6893,7 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="11" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B73" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6896,7 +6906,7 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="11" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B74" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6909,7 +6919,7 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="11" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B75" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6922,7 +6932,7 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="11" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B76" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6935,7 +6945,7 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="11" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B77" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6948,7 +6958,7 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="11" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B78" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6961,7 +6971,7 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="11" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B79" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6974,7 +6984,7 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="11" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B80" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6987,7 +6997,7 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="11" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B81" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7000,7 +7010,7 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="11" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B82" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7013,7 +7023,7 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="11" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B83" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7026,7 +7036,7 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="11" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B84" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7039,7 +7049,7 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="11" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B85" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7052,7 +7062,7 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="11" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B86" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7065,7 +7075,7 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="11" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B87" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7078,7 +7088,7 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="11" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B88" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7091,7 +7101,7 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="10" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B89" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7104,7 +7114,7 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="11" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B90" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7117,7 +7127,7 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="11" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B91" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7130,7 +7140,7 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="11" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B92" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7143,7 +7153,7 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="11" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B93" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7156,7 +7166,7 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="11" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B94" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7169,7 +7179,7 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="11" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B95" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7182,7 +7192,7 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="11" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B96" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7195,7 +7205,7 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="11" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B97" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7208,7 +7218,7 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="11" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B98" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7221,7 +7231,7 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="11" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B99" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7234,7 +7244,7 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="11" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B100" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7247,7 +7257,7 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="11" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B101" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7260,7 +7270,7 @@
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="11" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B102" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7273,7 +7283,7 @@
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="11" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B103" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7286,7 +7296,7 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="11" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B104" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7299,7 +7309,7 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="11" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B105" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7312,7 +7322,7 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="11" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B106" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7325,7 +7335,7 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="11" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B107" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7338,7 +7348,7 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="11" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B108" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7351,7 +7361,7 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="11" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B109" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7364,7 +7374,7 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="11" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B110" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7377,7 +7387,7 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="11" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B111" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7390,7 +7400,7 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="11" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B112" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7403,7 +7413,7 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="11" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B113" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7416,7 +7426,7 @@
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="11" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B114" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7429,7 +7439,7 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="11" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B115" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7442,7 +7452,7 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="11" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B116" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7455,7 +7465,7 @@
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="11" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B117" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7468,7 +7478,7 @@
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="11" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B118" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7481,7 +7491,7 @@
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="11" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B119" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7494,7 +7504,7 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="11" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B120" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7507,7 +7517,7 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="11" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B121" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7520,7 +7530,7 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="10" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B122" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7533,7 +7543,7 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="10" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B123" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7546,7 +7556,7 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="10" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B124" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7559,7 +7569,7 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="11" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B125" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7572,7 +7582,7 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="11" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B126" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7585,7 +7595,7 @@
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="11" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B127" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7598,7 +7608,7 @@
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="11" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B128" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7611,7 +7621,7 @@
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="11" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B129" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7624,7 +7634,7 @@
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="11" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B130" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7637,7 +7647,7 @@
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="10" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B131" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7650,7 +7660,7 @@
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="10" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B132" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7663,7 +7673,7 @@
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="11" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B133" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7676,7 +7686,7 @@
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="11" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="B134" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7689,7 +7699,7 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="11" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B135" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7702,7 +7712,7 @@
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="11" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B136" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7715,7 +7725,7 @@
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="11" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B137" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7728,7 +7738,7 @@
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="11" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B138" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7741,7 +7751,7 @@
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="11" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B139" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7754,7 +7764,7 @@
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="11" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B140" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7767,7 +7777,7 @@
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="11" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B141" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7780,7 +7790,7 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="11" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B142" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7793,7 +7803,7 @@
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="11" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B143" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7806,7 +7816,7 @@
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="11" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B144" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7819,7 +7829,7 @@
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="11" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B145" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7832,7 +7842,7 @@
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="11" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B146" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7845,7 +7855,7 @@
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="11" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B147" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7858,7 +7868,7 @@
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="11" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B148" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7871,7 +7881,7 @@
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="11" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B149" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7884,7 +7894,7 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="11" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B150" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7897,7 +7907,7 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="11" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B151" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7910,7 +7920,7 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="11" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B152" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7923,7 +7933,7 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="11" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B153" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7936,7 +7946,7 @@
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="11" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B154" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7949,7 +7959,7 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="11" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B155" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7962,7 +7972,7 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="11" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B156" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7975,7 +7985,7 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="11" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="B157" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7988,7 +7998,7 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="10" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B158" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8001,7 +8011,7 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="11" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B159" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8014,7 +8024,7 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="11" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B160" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8027,7 +8037,7 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="11" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B161" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8040,7 +8050,7 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="11" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B162" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8053,7 +8063,7 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="10" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="B163" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8066,7 +8076,7 @@
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="11" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B164" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8079,7 +8089,7 @@
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="10" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B165" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8092,7 +8102,7 @@
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="11" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="B166" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8105,7 +8115,7 @@
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="11" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B167" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8118,7 +8128,7 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="11" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B168" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8131,7 +8141,7 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="11" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B169" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8144,7 +8154,7 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="11" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="B170" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8157,7 +8167,7 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="10" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B171" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8170,7 +8180,7 @@
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="10" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B172" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8183,7 +8193,7 @@
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="11" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B173" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8196,7 +8206,7 @@
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="10" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B174" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8209,7 +8219,7 @@
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="11" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B175" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8222,7 +8232,7 @@
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="11" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B176" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8235,7 +8245,7 @@
     </row>
     <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="11" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B177" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8248,7 +8258,7 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="11" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B178" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8261,7 +8271,7 @@
     </row>
     <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="11" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B179" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8274,7 +8284,7 @@
     </row>
     <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="11" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B180" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8287,7 +8297,7 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="11" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B181" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8300,7 +8310,7 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="11" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B182" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8313,7 +8323,7 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="11" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B183" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8326,7 +8336,7 @@
     </row>
     <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="10" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B184" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8339,7 +8349,7 @@
     </row>
     <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="10" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B185" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8352,7 +8362,7 @@
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="11" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B186" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8365,7 +8375,7 @@
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="11" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B187" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8378,7 +8388,7 @@
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="11" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="B188" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8391,7 +8401,7 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="11" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B189" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8404,7 +8414,7 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="11" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B190" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8417,7 +8427,7 @@
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="11" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B191" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8430,7 +8440,7 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="11" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B192" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8443,7 +8453,7 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="11" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B193" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8456,7 +8466,7 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="11" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B194" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8469,7 +8479,7 @@
     </row>
     <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="10" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B195" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8482,7 +8492,7 @@
     </row>
     <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="11" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B196" s="11" t="str">
         <f t="shared" si="1"/>
@@ -8495,7 +8505,7 @@
     </row>
     <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="11" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B197" s="11" t="str">
         <f t="shared" si="1"/>
@@ -9342,7 +9352,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -9446,7 +9456,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>29</v>
@@ -9590,7 +9600,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>786</v>
+        <v>587</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>65</v>
@@ -10815,7 +10825,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B1" s="11" t="str">
         <f t="shared" ref="B1:B197" si="1">TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LEFT(A1, FIND(":", A1) - 1), """", ""), "'", ""), ",", ""))</f>
@@ -10828,7 +10838,7 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B2" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10841,7 +10851,7 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B3" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10854,7 +10864,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B4" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10867,7 +10877,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B5" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10880,7 +10890,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B6" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10893,7 +10903,7 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B7" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10906,7 +10916,7 @@
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B8" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10919,7 +10929,7 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B9" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10932,7 +10942,7 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B10" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10945,7 +10955,7 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B11" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10958,7 +10968,7 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B12" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10971,7 +10981,7 @@
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B13" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10984,7 +10994,7 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B14" s="11" t="str">
         <f t="shared" si="1"/>
@@ -10997,7 +11007,7 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B15" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11010,7 +11020,7 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B16" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11023,7 +11033,7 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B17" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11036,7 +11046,7 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B18" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11049,7 +11059,7 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B19" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11062,7 +11072,7 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B20" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11075,7 +11085,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B21" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11088,7 +11098,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B22" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11101,7 +11111,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B23" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11114,7 +11124,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B24" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11127,7 +11137,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B25" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11140,7 +11150,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B26" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11153,7 +11163,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B27" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11166,7 +11176,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B28" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11179,7 +11189,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B29" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11192,7 +11202,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B30" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11205,7 +11215,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B31" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11218,7 +11228,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B32" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11231,7 +11241,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B33" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11244,7 +11254,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B34" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11257,7 +11267,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B35" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11270,7 +11280,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B36" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11283,7 +11293,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B37" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11296,7 +11306,7 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B38" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11309,7 +11319,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B39" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11322,7 +11332,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B40" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11335,7 +11345,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B41" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11348,7 +11358,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B42" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11361,7 +11371,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="11" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B43" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11374,7 +11384,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="11" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B44" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11387,7 +11397,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B45" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11400,7 +11410,7 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B46" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11413,7 +11423,7 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B47" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11426,7 +11436,7 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="11" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B48" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11439,7 +11449,7 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="11" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B49" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11452,7 +11462,7 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B50" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11465,7 +11475,7 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="11" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B51" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11478,7 +11488,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="11" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B52" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11491,7 +11501,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="11" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B53" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11504,7 +11514,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="11" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B54" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11517,7 +11527,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="11" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B55" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11530,7 +11540,7 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="11" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B56" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11543,7 +11553,7 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="11" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B57" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11556,7 +11566,7 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="11" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B58" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11569,7 +11579,7 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="11" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B59" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11582,7 +11592,7 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="10" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B60" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11595,7 +11605,7 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="11" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B61" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11608,7 +11618,7 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="10" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B62" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11621,7 +11631,7 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="11" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B63" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11634,7 +11644,7 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="11" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B64" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11647,7 +11657,7 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="11" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B65" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11660,7 +11670,7 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="11" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B66" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11673,7 +11683,7 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B67" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11686,7 +11696,7 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="11" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B68" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11699,7 +11709,7 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="11" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="B69" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11712,7 +11722,7 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="11" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B70" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11725,7 +11735,7 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="11" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B71" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11738,7 +11748,7 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="11" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B72" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11751,7 +11761,7 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="11" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B73" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11764,7 +11774,7 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="11" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B74" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11777,7 +11787,7 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="11" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B75" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11790,7 +11800,7 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="11" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B76" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11803,7 +11813,7 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="11" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B77" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11816,7 +11826,7 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="11" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B78" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11829,7 +11839,7 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="11" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B79" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11842,7 +11852,7 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="11" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B80" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11855,7 +11865,7 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="11" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B81" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11868,7 +11878,7 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="11" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B82" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11881,7 +11891,7 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="11" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B83" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11894,7 +11904,7 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="11" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B84" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11907,7 +11917,7 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="11" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B85" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11920,7 +11930,7 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="11" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B86" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11933,7 +11943,7 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="11" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B87" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11946,7 +11956,7 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="11" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B88" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11959,7 +11969,7 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="10" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B89" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11972,7 +11982,7 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="11" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B90" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11985,7 +11995,7 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="11" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B91" s="11" t="str">
         <f t="shared" si="1"/>
@@ -11998,7 +12008,7 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="11" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B92" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12011,7 +12021,7 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="11" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B93" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12024,7 +12034,7 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="11" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B94" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12037,7 +12047,7 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="11" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B95" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12050,7 +12060,7 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="11" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B96" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12063,7 +12073,7 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="11" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B97" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12076,7 +12086,7 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="11" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B98" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12089,7 +12099,7 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="11" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B99" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12102,7 +12112,7 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="11" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B100" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12115,7 +12125,7 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="11" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B101" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12128,7 +12138,7 @@
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="11" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B102" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12141,7 +12151,7 @@
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="11" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B103" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12154,7 +12164,7 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="11" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B104" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12167,7 +12177,7 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="11" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B105" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12180,7 +12190,7 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="11" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B106" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12193,7 +12203,7 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="11" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B107" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12206,7 +12216,7 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="11" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B108" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12219,7 +12229,7 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="11" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B109" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12232,7 +12242,7 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="11" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B110" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12245,7 +12255,7 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="11" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B111" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12258,7 +12268,7 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="11" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B112" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12271,7 +12281,7 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="11" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B113" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12284,7 +12294,7 @@
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="11" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B114" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12297,7 +12307,7 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="11" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B115" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12310,7 +12320,7 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="11" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B116" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12323,7 +12333,7 @@
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="11" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B117" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12336,7 +12346,7 @@
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="11" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B118" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12349,7 +12359,7 @@
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="11" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B119" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12362,7 +12372,7 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="11" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B120" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12375,7 +12385,7 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="11" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B121" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12388,7 +12398,7 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="10" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B122" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12401,7 +12411,7 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="10" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B123" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12414,7 +12424,7 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="10" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B124" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12427,7 +12437,7 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="11" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B125" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12440,7 +12450,7 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="11" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B126" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12453,7 +12463,7 @@
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="11" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B127" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12466,7 +12476,7 @@
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="11" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B128" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12479,7 +12489,7 @@
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="11" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B129" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12492,7 +12502,7 @@
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="11" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B130" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12505,7 +12515,7 @@
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="10" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B131" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12518,7 +12528,7 @@
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="10" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B132" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12531,7 +12541,7 @@
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="11" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B133" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12544,7 +12554,7 @@
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="11" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="B134" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12557,7 +12567,7 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="11" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B135" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12570,7 +12580,7 @@
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="11" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B136" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12583,7 +12593,7 @@
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="11" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B137" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12596,7 +12606,7 @@
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="11" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B138" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12609,7 +12619,7 @@
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="11" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B139" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12622,7 +12632,7 @@
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="11" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B140" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12635,7 +12645,7 @@
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="11" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B141" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12648,7 +12658,7 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="11" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B142" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12661,7 +12671,7 @@
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="11" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B143" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12674,7 +12684,7 @@
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="11" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B144" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12687,7 +12697,7 @@
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="11" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B145" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12700,7 +12710,7 @@
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="11" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B146" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12713,7 +12723,7 @@
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="11" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B147" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12726,7 +12736,7 @@
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="11" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B148" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12739,7 +12749,7 @@
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="11" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B149" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12752,7 +12762,7 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="11" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B150" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12765,7 +12775,7 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="11" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B151" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12778,7 +12788,7 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="11" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B152" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12791,7 +12801,7 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="11" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B153" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12804,7 +12814,7 @@
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="11" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B154" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12817,7 +12827,7 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="11" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B155" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12830,7 +12840,7 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="11" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B156" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12843,7 +12853,7 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="11" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="B157" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12856,7 +12866,7 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="10" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B158" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12869,7 +12879,7 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="11" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B159" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12882,7 +12892,7 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="11" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B160" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12895,7 +12905,7 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="11" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B161" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12908,7 +12918,7 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="11" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B162" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12921,7 +12931,7 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="10" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="B163" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12934,7 +12944,7 @@
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="11" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B164" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12947,7 +12957,7 @@
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="10" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B165" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12960,7 +12970,7 @@
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="11" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="B166" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12973,7 +12983,7 @@
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="11" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B167" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12986,7 +12996,7 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="11" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B168" s="11" t="str">
         <f t="shared" si="1"/>
@@ -12999,7 +13009,7 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="11" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B169" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13012,7 +13022,7 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="11" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="B170" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13025,7 +13035,7 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="10" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B171" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13038,7 +13048,7 @@
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="10" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B172" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13051,7 +13061,7 @@
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="11" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B173" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13064,7 +13074,7 @@
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="10" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B174" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13077,7 +13087,7 @@
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="11" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B175" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13090,7 +13100,7 @@
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="11" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B176" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13103,7 +13113,7 @@
     </row>
     <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="11" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B177" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13116,7 +13126,7 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="11" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B178" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13129,7 +13139,7 @@
     </row>
     <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="11" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B179" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13142,7 +13152,7 @@
     </row>
     <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="11" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B180" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13155,7 +13165,7 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="11" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B181" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13168,7 +13178,7 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="11" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B182" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13181,7 +13191,7 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="11" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B183" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13194,7 +13204,7 @@
     </row>
     <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="10" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B184" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13207,7 +13217,7 @@
     </row>
     <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="10" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B185" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13220,7 +13230,7 @@
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="11" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B186" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13233,7 +13243,7 @@
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="11" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B187" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13246,7 +13256,7 @@
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="11" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="B188" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13259,7 +13269,7 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="11" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B189" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13272,7 +13282,7 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="11" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B190" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13285,7 +13295,7 @@
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="11" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B191" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13298,7 +13308,7 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="11" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B192" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13311,7 +13321,7 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="11" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B193" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13324,7 +13334,7 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="11" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B194" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13337,7 +13347,7 @@
     </row>
     <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="10" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B195" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13350,7 +13360,7 @@
     </row>
     <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="11" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B196" s="11" t="str">
         <f t="shared" si="1"/>
@@ -13363,7 +13373,7 @@
     </row>
     <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="11" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B197" s="11" t="str">
         <f t="shared" si="1"/>

</xml_diff>